<commit_message>
import script working unit tests in progress
</commit_message>
<xml_diff>
--- a/tests/files/import_attainments_corrupt_base_subject.xlsx
+++ b/tests/files/import_attainments_corrupt_base_subject.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GM/Code/test-correct/tests/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938C1CA1-92B7-374D-B1D0-83B051C3DDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C965EE2-E6DD-AE4F-A8F8-7A81F14EFDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="460" windowWidth="27640" windowHeight="16940" xr2:uid="{8D80483A-517E-4D4B-A5DE-468943674C88}"/>
+    <workbookView xWindow="4320" yWindow="460" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{8D80483A-517E-4D4B-A5DE-468943674C88}"/>
   </bookViews>
   <sheets>
     <sheet name="Aardrijkskunde" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3480" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3481" uniqueCount="425">
   <si>
     <t>Table 1</t>
   </si>
@@ -1839,7 +1839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5437FBD-7CD4-FE4D-B98B-5075F44E0662}">
   <dimension ref="A1:P318"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -13227,8 +13227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1EBCCF0-2BAB-704F-965C-055D67A37A60}">
   <dimension ref="A1:P354"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -13285,7 +13285,9 @@
       <c r="H2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="19"/>
+      <c r="I2" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="J2" s="19" t="s">
         <v>10</v>
       </c>

</xml_diff>